<commit_message>
Idk what I have changed
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\PetrolTrulyUnlimited\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3A790C-07EA-4597-913D-E920925C6034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587E659C-6D5A-4AE3-911F-FFFAC701BE08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C28777FE-C02A-449A-86E0-F4A180F0544D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
   <si>
     <t>Petrol Truly Unlimited</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Try to write data that isn't supposed to be on the textbox</t>
   </si>
   <si>
-    <t>Close program after at least one vehicle finnishes fuelling</t>
-  </si>
-  <si>
     <t>Vehicles dont take more than the maximum fueling time</t>
   </si>
   <si>
@@ -247,6 +244,57 @@
   </si>
   <si>
     <t>The vehicle leavs the pump making it available</t>
+  </si>
+  <si>
+    <t>After the vehicle leaves the receipt is saved</t>
+  </si>
+  <si>
+    <t>Wait for a vehicle leaves the pump and look for a receipt</t>
+  </si>
+  <si>
+    <t>A new receipt is saved</t>
+  </si>
+  <si>
+    <t>Pumps information is updated</t>
+  </si>
+  <si>
+    <t>Everytime a vehicle enters or leaved the stats is updated</t>
+  </si>
+  <si>
+    <t>Each car is spawned with random information</t>
+  </si>
+  <si>
+    <t>Move the mouse over the pump to see the statistics of each pump</t>
+  </si>
+  <si>
+    <t>Move the mouse over the vehicle to see the information of each vehicle</t>
+  </si>
+  <si>
+    <t>A popup should appear with the vehicle information</t>
+  </si>
+  <si>
+    <t>The queue should have information updated everytime</t>
+  </si>
+  <si>
+    <t>Move the mouse over the queue to see the statistics</t>
+  </si>
+  <si>
+    <t>A popup should appear with the queue information</t>
+  </si>
+  <si>
+    <t>Each car in the pump should open a popup with information about the vehicle</t>
+  </si>
+  <si>
+    <t>Move the mouse over the car that is in the pump</t>
+  </si>
+  <si>
+    <t>Should be possible to scroll through the last 200 receipts</t>
+  </si>
+  <si>
+    <t>When the receipt list has enough items a scroll bar should appear and we it should be able to scroll</t>
+  </si>
+  <si>
+    <t>List should be able to scroll</t>
   </si>
 </sst>
 </file>
@@ -648,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96167F48-34D8-4B94-8371-FDC101FE25AA}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +758,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -1013,13 +1061,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>8</v>
@@ -1030,13 +1078,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
@@ -1047,71 +1095,119 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">

</xml_diff>